<commit_message>
api added for register help
</commit_message>
<xml_diff>
--- a/Backend/APIs.xlsx
+++ b/Backend/APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BtB_RuntimeTerror\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08C8CAC-4E84-4F44-8B5A-B4EA1B8F392F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB9D38A-596D-4C3B-B22F-0FC4DB21AD5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D54B11D4-4C1F-430C-ABA5-6C960AEF182D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>API Endpoint</t>
   </si>
@@ -36,15 +36,9 @@
     <t>/api/user/signup</t>
   </si>
   <si>
-    <t>/api/user/updatedetails</t>
-  </si>
-  <si>
     <t>/api/ngo/signup</t>
   </si>
   <si>
-    <t>/api/ngo/updatedetails</t>
-  </si>
-  <si>
     <t>/api/ngo/list</t>
   </si>
   <si>
@@ -63,13 +57,58 @@
     <t>UserTypeId, email, password</t>
   </si>
   <si>
-    <t>{"Id" :  1, userdetails: {}, addressdetails : {}, verificationdetails : {}</t>
-  </si>
-  <si>
     <t>/api/login</t>
   </si>
   <si>
     <t>email,password</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Create account for user</t>
+  </si>
+  <si>
+    <t>Create account for NGOs</t>
+  </si>
+  <si>
+    <t>update all details of user</t>
+  </si>
+  <si>
+    <t>update all details of NGOs</t>
+  </si>
+  <si>
+    <t>returns  list of  all active NGOs</t>
+  </si>
+  <si>
+    <t>login for user or NGO</t>
+  </si>
+  <si>
+    <t>/api/offeredhelps</t>
+  </si>
+  <si>
+    <t>/api/user/offeredhelps/:userid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list all user offered helps </t>
+  </si>
+  <si>
+    <t>get all helps offered by the given user</t>
+  </si>
+  <si>
+    <t>{userdetails: {}, addressdetails : {}, verificationdetails : {}</t>
+  </si>
+  <si>
+    <t>/api/user/updatedetails/:userid</t>
+  </si>
+  <si>
+    <t>/api/ngo/updatedetails/:userid</t>
+  </si>
+  <si>
+    <t>/api/user/offeringhelp/:userid</t>
+  </si>
+  <si>
+    <t>register help</t>
   </si>
 </sst>
 </file>
@@ -441,22 +480,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2F082C-9926-4605-BBF9-379DF81A9C12}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -464,70 +503,124 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
+      <c r="C11" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get user profile detail api added
</commit_message>
<xml_diff>
--- a/Backend/APIs.xlsx
+++ b/Backend/APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BtB_RuntimeTerror\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB9D38A-596D-4C3B-B22F-0FC4DB21AD5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D49D688-F8F1-4930-A0A7-841FC18B0007}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D54B11D4-4C1F-430C-ABA5-6C960AEF182D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>API Endpoint</t>
   </si>
@@ -87,9 +87,6 @@
     <t>/api/offeredhelps</t>
   </si>
   <si>
-    <t>/api/user/offeredhelps/:userid</t>
-  </si>
-  <si>
     <t xml:space="preserve">list all user offered helps </t>
   </si>
   <si>
@@ -109,6 +106,15 @@
   </si>
   <si>
     <t>register help</t>
+  </si>
+  <si>
+    <t>/api/user/offeredhelp/:userid</t>
+  </si>
+  <si>
+    <t>/api/user/profiledetails/:userid</t>
+  </si>
+  <si>
+    <t>get all user details</t>
   </si>
 </sst>
 </file>
@@ -480,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2F082C-9926-4605-BBF9-379DF81A9C12}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +531,7 @@
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -534,7 +540,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -553,7 +559,7 @@
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -562,7 +568,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -598,29 +604,40 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get ngo profile details Api added
</commit_message>
<xml_diff>
--- a/Backend/APIs.xlsx
+++ b/Backend/APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BtB_RuntimeTerror\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D49D688-F8F1-4930-A0A7-841FC18B0007}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD83E2D-7E37-4552-B977-18FA40654756}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D54B11D4-4C1F-430C-ABA5-6C960AEF182D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>API Endpoint</t>
   </si>
@@ -114,7 +114,13 @@
     <t>/api/user/profiledetails/:userid</t>
   </si>
   <si>
-    <t>get all user details</t>
+    <t>/api/ngo/profiledetails/:userid</t>
+  </si>
+  <si>
+    <t>get all details of ngo</t>
+  </si>
+  <si>
+    <t>get all details user</t>
   </si>
 </sst>
 </file>
@@ -486,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2F082C-9926-4605-BBF9-379DF81A9C12}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +643,18 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
verify user and ngo API added
</commit_message>
<xml_diff>
--- a/Backend/APIs.xlsx
+++ b/Backend/APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BtB_RuntimeTerror\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD83E2D-7E37-4552-B977-18FA40654756}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14706D54-A67A-4707-A37C-34EB52007CBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D54B11D4-4C1F-430C-ABA5-6C960AEF182D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>API Endpoint</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>get all details user</t>
+  </si>
+  <si>
+    <t>/api/ngo/:ngoid/verify/:userid</t>
+  </si>
+  <si>
+    <t>verify user</t>
+  </si>
+  <si>
+    <t>/api/user/:userid/verify/:ngoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify NGO </t>
   </si>
 </sst>
 </file>
@@ -492,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2F082C-9926-4605-BBF9-379DF81A9C12}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,6 +669,28 @@
         <v>30</v>
       </c>
     </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
API's added and unit test cases
</commit_message>
<xml_diff>
--- a/Backend/APIs.xlsx
+++ b/Backend/APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BtB_RuntimeTerror\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475AAC92-BAC4-480A-8A93-EDAB4D2131AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04078209-CEF0-4103-8192-EAABFC0E23E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D54B11D4-4C1F-430C-ABA5-6C960AEF182D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>API Endpoint</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>add government shelters</t>
+  </si>
+  <si>
+    <t>/ngo/:email</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>/user/:email</t>
   </si>
 </sst>
 </file>
@@ -516,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2F082C-9926-4605-BBF9-379DF81A9C12}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,6 +735,22 @@
         <v>39</v>
       </c>
     </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added api and unit tests
</commit_message>
<xml_diff>
--- a/Backend/APIs.xlsx
+++ b/Backend/APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BtB_RuntimeTerror\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04078209-CEF0-4103-8192-EAABFC0E23E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343D04B5-6082-4CC2-84B0-AD081297A21C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D54B11D4-4C1F-430C-ABA5-6C960AEF182D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>API Endpoint</t>
   </si>
@@ -147,13 +147,25 @@
     <t>add government shelters</t>
   </si>
   <si>
-    <t>/ngo/:email</t>
-  </si>
-  <si>
     <t>delete</t>
   </si>
   <si>
-    <t>/user/:email</t>
+    <t>/api/ngo/:email</t>
+  </si>
+  <si>
+    <t>/api/user/:email</t>
+  </si>
+  <si>
+    <t>/api/unverifiedusers</t>
+  </si>
+  <si>
+    <t>list of unverified users</t>
+  </si>
+  <si>
+    <t>delete the ngo</t>
+  </si>
+  <si>
+    <t>delete the user</t>
   </si>
 </sst>
 </file>
@@ -525,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2F082C-9926-4605-BBF9-379DF81A9C12}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,10 +749,13 @@
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" t="s">
-        <v>41</v>
+      <c r="C18" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -748,7 +763,21 @@
         <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>